<commit_message>
Added saline eCAMI sig cazyme; updated sig cazyme ECs
</commit_message>
<xml_diff>
--- a/dbcan/sig_cazy_info.xlsx
+++ b/dbcan/sig_cazy_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/dbcan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="372" documentId="8_{A1E0EE2A-CA9E-4781-BABE-4A2888B05358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C22F1F9-FDBC-489C-B43D-4962F57136F6}"/>
+  <xr:revisionPtr revIDLastSave="500" documentId="8_{A1E0EE2A-CA9E-4781-BABE-4A2888B05358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9A162C0-69B0-455E-A0B8-E99381AF76D1}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{88FD4827-B98C-4388-B407-BA95E8DEB523}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{88FD4827-B98C-4388-B407-BA95E8DEB523}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="99">
   <si>
     <t>CAZyme</t>
   </si>
@@ -159,12 +159,6 @@
   </si>
   <si>
     <t>acetyl xylan esterase (EC 3.1.1.72)</t>
-  </si>
-  <si>
-    <t>Tons of ECs</t>
-  </si>
-  <si>
-    <t>CAZyme Info</t>
   </si>
   <si>
     <t xml:space="preserve">endo-B-N-acetylglucosaminidase (EC 3.2.1.96)
@@ -200,15 +194,6 @@
 rhamnogalacturonan exolyase (EC 4.2.2.24)</t>
   </si>
   <si>
-    <t>Tons of Ecs. Potential mucin deg</t>
-  </si>
-  <si>
-    <t>Tons of ECs. Portential mucin deg</t>
-  </si>
-  <si>
-    <t>Potential mucin deg</t>
-  </si>
-  <si>
     <t>Mucin deg</t>
   </si>
   <si>
@@ -241,25 +226,212 @@
 chitinase (EC 3.2.1.14)</t>
   </si>
   <si>
-    <t xml:space="preserve">N-acetyl B-glucosaminidase (EC 3.2.1.52)
-hyaluronidase (EC 3.2.1.35)
-[protein]-3-O-(GlcNAc)-L-Ser/Thr B-N-acetylglucosaminidase (EC 3.2.1.169)
-</t>
-  </si>
-  <si>
-    <t>Tons of Ecs</t>
-  </si>
-  <si>
     <t>B-xylosidase (EC 3.2.1.37)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>3.2.1.52</t>
+  </si>
+  <si>
+    <t>4.2.2.N1</t>
+  </si>
+  <si>
+    <t>3.2.1.18</t>
+  </si>
+  <si>
+    <t>3.2.1.23</t>
+  </si>
+  <si>
+    <t>3.2.1.37
+3.2.1.55</t>
+  </si>
+  <si>
+    <t>3.2.1.55</t>
+  </si>
+  <si>
+    <t>3.2.1.169
+3.2.1.35</t>
+  </si>
+  <si>
+    <t>3.2.1.91
+3.2.1.176
+3.2.1.4
+3.2.1.151
+3.2.1.14
+3.2.1.73</t>
+  </si>
+  <si>
+    <t>2.4.1.280
+2.4.1.20</t>
+  </si>
+  <si>
+    <t>2.4.1.11
+2.4.1.1</t>
+  </si>
+  <si>
+    <t>4.2.2.23
+4.2.2.24</t>
+  </si>
+  <si>
+    <t>4.2.2.23
+4.2.2.24
+3.1.1.11
+3.1.1.86
+1.1.1.40
+1.1.1.38
+1.1.1.169
+1.1.1.39</t>
+  </si>
+  <si>
+    <t>3.2.1.8
+3.2.1.4
+3.2.1.55
+3.2.1.91
+3.1.1.73
+3.2.1.78
+3.2.1.91</t>
+  </si>
+  <si>
+    <t>1.1.1.292
+1.1.1.18
+1.1.1.369
+1.1.1.371
+1.1.1.361</t>
+  </si>
+  <si>
+    <t>Overlap</t>
   </si>
   <si>
     <t>pectin acetylesterase
 rhamnogalacturonan acetylesterase
-acetyl xylan esterase
-3.1.1.- or 3.1.1.72</t>
-  </si>
-  <si>
-    <t>glycogen synthase (EC 2.4.11)</t>
+acetyl xylan esterase</t>
+  </si>
+  <si>
+    <t>Transglycosylase (EC 4.2.2.N1)</t>
+  </si>
+  <si>
+    <t>B-galactosidase (EC 3.2.1.23)</t>
+  </si>
+  <si>
+    <t>hyaluronidase (3.2.1.35)
+acetylglucosaminidase (EC 3.2.1.169)</t>
+  </si>
+  <si>
+    <t>glycogen synthase (EC 2.4.1.11)</t>
+  </si>
+  <si>
+    <t>β-glucosidase (EC 3.2.1.21)
+xylan 1,4-β-xylosidase (EC 3.2.1.37)
+β-glucosylceramidase (EC 3.2.1.45)
+β-N-acetylhexosaminidase (EC 3.2.1.52)
+α-L-arabinofuranosidase (EC 3.2.1.55)
+glucan 1,4-β-glucosidase (EC 3.2.1.74)
+isoprimeverose-producing oligoxyloglucan hydrolase (EC 3.2.1.120)
+coniferin β-glucosidase (EC 3.2.1.126)
+xyloglucan-specific exo-β-1,4-glucanase / exo-xyloglucanase (EC 3.2.1.155)
+lichenase / endo-β-1,3-1,4-glucanase (EC 3.2.1.73)
+protodioscin 26-O-β-D-glucosidase (EC 3.2.1.186)
+β-glucuronidase (EC 3.2.1.31)</t>
+  </si>
+  <si>
+    <t>3.2.1.21
+3.2.1.37
+3.2.1.55
+3.2.1.52
+1.5.1.6
+3.6.1.3</t>
+  </si>
+  <si>
+    <t>β-glucosidase (EC 3.2.1.21)
+xylan 1,4-β-xylosidase (EC 3.2.1.37)
+β-N-acetylhexosaminidase (EC 3.2.1.52)
+α-L-arabinofuranosidase (EC 3.2.1.55)</t>
+  </si>
+  <si>
+    <t>endoglucanase (EC 3.2.1.4)
+endo-β-1,3(4)-glucanase / lichenase-laminarinase (EC 3.2.1.6)
+lichenase / endo-β-1,3-1,4-glucanase (EC 3.2.1.73)
+exo-β-1,4-glucanase / cellodextrinase (EC 3.2.1.74)
+cellobiohydrolase (EC 3.2.1.91)
+xyloglucan-specific endo-β-1,4-glucanase / endo-xyloglucanase (EC 3.2.1.151)
+exo-β-glucosaminidase (EC 3.2.1.165)</t>
+  </si>
+  <si>
+    <t>endoglucanase (EC 3.2.1.4)
+lichenase / endo-β-1,3-1,4-glucanase (EC 3.2.1.73)
+cellobiohydrolase (EC 3.2.1.91)
+xyloglucan-specific endo-β-1,4-glucanase / endo-xyloglucanase (EC 3.2.1.151)</t>
+  </si>
+  <si>
+    <t>endo-1,4-β-xylanase (EC 3.2.1.8)
+endo-1,3-β-xylanase (EC 3.2.1.32)
+endo-β-1,4-glucanase (EC 3.2.1.4)</t>
+  </si>
+  <si>
+    <t>endo-β-1,4-glucanase (EC 3.2.1.4)
+endo-1,4-β-xylanase (EC 3.2.1.8)</t>
+  </si>
+  <si>
+    <t>α-glucosidase (EC 3.2.1.20)
+α-galactosidase (EC 3.2.1.22)
+α-mannosidase (EC 3.2.1.24)
+α-1,3-glucosidase (EC 3.2.1.84)
+sucrase-isomaltase (EC 3.2.1.48) (EC 3.2.1.10)
+α-xylosidase (EC 3.2.1.177)
+α-glucan lyase (EC 4.2.2.13)
+oligosaccharide α-1,4-glucosyltransferase (EC 2.4.1.161)
+α-N-acetylgalactosaminidase (EC 3.2.1.49)
+sulfoquinovosidase (EC 3.2.1.199)
+α-6-glucosyltransferase (EC 2.4.1.24)</t>
+  </si>
+  <si>
+    <t>α-glucosidase (EC 3.2.1.20)
+α-1,3-glucosidase (EC 3.2.1.84)
+α-xylosidase (EC 3.2.1.177)</t>
+  </si>
+  <si>
+    <t>3.2.1.177
+3.2.1.84
+3.2.1.20</t>
+  </si>
+  <si>
+    <t>sialidase or neuraminidase (EC 3.2.1.18)
+anhydrosialidase (EC 4.2.2.15)</t>
+  </si>
+  <si>
+    <t>endoglucanase (EC 3.2.1.4)
+endo-β-1,4-xylanase (EC 3.2.1.8)
+β-xylosidase (EC 3.2.1.37)
+α-L-arabinofuranosidase (EC 3.2.1.55)
+cellobiohydrolase (EC 3.2.1.91)</t>
+  </si>
+  <si>
+    <t>α-L-arabinofuranosidase (EC 3.2.1.55)</t>
+  </si>
+  <si>
+    <t>N-acetyl B-glucosaminidase (EC 3.2.1.52)
+hyaluronidase (EC 3.2.1.35)
+[protein]-3-O-(GlcNAc)-L-Ser/Thr B-N-acetylglucosaminidase (EC 3.2.1.169)</t>
+  </si>
+  <si>
+    <t>cellobiose phosphorylase (EC 2.4.1.20)
+laminaribiose phosphorylase (EC 2.4.1.31)
+cellodextrin phosphorylase (EC 2.4.1.49)
+chitobiose phosphorylase (EC 2.4.1.280)
+cellobionic acid phosphorylase (EC 2.4.1.321)
+β-1,2-oligoglucan phosphorylase (EC 2.4.1.333)</t>
+  </si>
+  <si>
+    <t>cellobiose phosphorylase (EC 2.4.1.20)
+chitobiose phosphorylase (EC 2.4.1.280)</t>
+  </si>
+  <si>
+    <t>CAZyme Full EC</t>
+  </si>
+  <si>
+    <t>Function</t>
   </si>
 </sst>
 </file>
@@ -328,7 +500,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -647,14 +819,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0420F783-523D-474B-9879-99329AEC3FC0}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:I24"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
-    <col min="5" max="5" width="49.7109375" customWidth="1"/>
+    <col min="4" max="5" width="49.7109375" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -669,10 +840,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -697,48 +868,66 @@
       <c r="B2" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="E2" s="4" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>52</v>
+      <c r="C4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -748,39 +937,54 @@
       <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>41</v>
+      <c r="C5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>41</v>
+      <c r="C6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>41</v>
+      <c r="C7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>36</v>
@@ -793,8 +997,11 @@
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>51</v>
+      <c r="C8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>35</v>
@@ -802,27 +1009,39 @@
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="E9" s="4" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>51</v>
+      <c r="C10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>36</v>
@@ -835,8 +1054,8 @@
       <c r="B11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>51</v>
+      <c r="C11" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>35</v>
@@ -849,25 +1068,34 @@
       <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>53</v>
+      <c r="C12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>41</v>
+      <c r="C13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>36</v>
@@ -880,22 +1108,34 @@
       <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="E14" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>41</v>
+      <c r="C15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>36</v>
@@ -903,50 +1143,59 @@
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>65</v>
+      <c r="C16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>53</v>
+      <c r="C17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>54</v>
+      <c r="C18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>35</v>
@@ -959,39 +1208,51 @@
       <c r="B19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>51</v>
+      <c r="C19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>41</v>
+      <c r="C20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>53</v>
+      <c r="C21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>35</v>
@@ -1004,8 +1265,14 @@
       <c r="B22" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="E22" s="4" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>36</v>
@@ -1013,27 +1280,39 @@
     </row>
     <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="C23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="E23" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="C24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="E24" s="4" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>29</v>
@@ -1046,8 +1325,14 @@
       <c r="B25" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="E25" s="4" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>36</v>
@@ -1060,8 +1345,14 @@
       <c r="B26" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="E26" s="4" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>36</v>
@@ -1074,8 +1365,11 @@
       <c r="B27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>41</v>
+      <c r="C27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>27</v>
@@ -1088,8 +1382,14 @@
       <c r="B28" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="E28" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>36</v>
@@ -1097,25 +1397,31 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E19904D-E189-4D84-A406-27FFA4DB4AA2}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1123,31 +1429,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1155,77 +1455,65 @@
         <v>34</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="3"/>
+      <c r="C3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="3"/>
+      <c r="C4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>44</v>
+      <c r="C5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1233,18 +1521,14 @@
         <v>34</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1253,36 +1537,30 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="4" t="s">
-        <v>45</v>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
@@ -1291,17 +1569,13 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1310,17 +1584,13 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="4" t="s">
-        <v>48</v>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="H10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1329,17 +1599,13 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="4" t="s">
-        <v>67</v>
+      <c r="E11" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="H11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -1348,106 +1614,90 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="3"/>
+      <c r="C14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="3"/>
+      <c r="C15" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="3"/>
+      <c r="C16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="4" t="s">
-        <v>66</v>
+      <c r="E17" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -1456,17 +1706,13 @@
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="4" t="s">
-        <v>40</v>
+      <c r="E18" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1474,19 +1720,15 @@
         <v>37</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H22" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1495,20 +1737,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB10AEF-13C5-47BF-802B-88E09E3AE0CB}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1516,31 +1757,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1548,18 +1783,14 @@
         <v>38</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1567,38 +1798,30 @@
         <v>38</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
+      <c r="C4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -1607,21 +1830,15 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1629,58 +1846,46 @@
         <v>38</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="4" t="s">
-        <v>63</v>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -1688,38 +1893,32 @@
         <v>39</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="4" t="s">
-        <v>68</v>
+      <c r="E10" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H13" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated w/ eCAMI results!
</commit_message>
<xml_diff>
--- a/dbcan/sig_cazy_info.xlsx
+++ b/dbcan/sig_cazy_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/dbcan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="500" documentId="8_{A1E0EE2A-CA9E-4781-BABE-4A2888B05358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9A162C0-69B0-455E-A0B8-E99381AF76D1}"/>
+  <xr:revisionPtr revIDLastSave="620" documentId="8_{A1E0EE2A-CA9E-4781-BABE-4A2888B05358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC8B2B1B-0CBF-4A1F-AA40-A69AB1E5C289}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{88FD4827-B98C-4388-B407-BA95E8DEB523}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{88FD4827-B98C-4388-B407-BA95E8DEB523}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="122">
   <si>
     <t>CAZyme</t>
   </si>
@@ -302,11 +302,6 @@
   </si>
   <si>
     <t>Overlap</t>
-  </si>
-  <si>
-    <t>pectin acetylesterase
-rhamnogalacturonan acetylesterase
-acetyl xylan esterase</t>
   </si>
   <si>
     <t>Transglycosylase (EC 4.2.2.N1)</t>
@@ -428,17 +423,142 @@
 chitobiose phosphorylase (EC 2.4.1.280)</t>
   </si>
   <si>
-    <t>CAZyme Full EC</t>
-  </si>
-  <si>
     <t>Function</t>
+  </si>
+  <si>
+    <t>CAZyme entry (if no overlapped function)</t>
+  </si>
+  <si>
+    <t>pectin acetylesterase (EC 3.1.1.-)
+rhamnogalacturonan acetylesterase (EC 3.1.1.-)
+acetyl xylan esterase (EC 3.1.1.72)</t>
+  </si>
+  <si>
+    <t>endo-β-1,4-glucanase / cellulase (EC 3.2.1.4)
+endo-β-1,4-xylanase (EC 3.2.1.8)
+β-glucosidase (EC 3.2.1.21)
+β-mannosidase (EC 3.2.1.25)
+β-glucosylceramidase (EC 3.2.1.45)
+glucan β-1,3-glucosidase (EC 3.2.1.58)
+exo-β-1,4-glucanase / cellodextrinase (EC 3.2.1.74)
+glucan endo-1,6-β-glucosidase (EC 3.2.1.75)
+mannan endo-β-1,4-mannosidase (EC 3.2.1.78)
+cellulose β-1,4-cellobiosidase (EC 3.2.1.91)
+steryl β-glucosidase (EC 3.2.1.104)
+endoglycoceramidase (EC 3.2.1.123)
+β-primeverosidase (EC 3.2.1.149)
+xyloglucan-specific endo-β-1,4-glucanase (EC 3.2.1.151)
+endo-β-1,6-galactanase (EC 3.2.1.164)
+β-1,3-mannanase (EC 3.2.1.-)
+arabinoxylan-specific endo-β-1,4-xylanase (EC 3.2.1.-)
+mannan transglycosylase (EC 2.4.1.-)
+lichenase / endo-β-1,3-1,4-glucanase (EC 3.2.1.73)
+β-glycosidase (EC 3.2.1.-)
+endo-β-1,3-glucanase / laminarinase (EC 3.2.1.39)
+β-N-acetylhexosaminidase (EC 3.2.1.52)
+chitosanase (EC 3.2.1.132)
+β-D-galactofuranosidase (EC 3.2.1.146)
+β-galactosylceramidase (EC 3.2.1.46)
+β-rutinosidase /α-L-rhamnose-(1,6)-β-D-glucosidase (EC 3.2.1.-)
+α-L-arabinofuranosidase (EC 3.2.1.55)
+glucomannan-specific endo-β-1,4-glucanase (EC 3.2.1.-)
+hesperidin 6-O-α-L-rhamnosyl-β-glucosidase (EC 3.2.1.168)</t>
+  </si>
+  <si>
+    <t>β-hexosaminidase (EC 3.2.1.52)
+lacto-N-biosidase (EC 3.2.1.140)
+β-1,6-N-acetylglucosaminidase (EC 3.2.1.-)
+β-6-SO3-N-acetylglucosaminidase (EC 3.2.1.-)</t>
+  </si>
+  <si>
+    <t>β-hexosaminidase (EC 3.2.1.52)</t>
+  </si>
+  <si>
+    <t>sialidase or neuraminidase (EC 3.2.1.18)
+trans-sialidase (EC 2.4.1.-)
+anhydrosialidase (EC 4.2.2.15)
+Kdo hydrolase (EC 3.2.1.-)
+2-keto-3-deoxynononic acid hydrolase / KDNase (EC 3.2.1.-)</t>
+  </si>
+  <si>
+    <t>sialidase or neuraminidase (EC 3.2.1.18)</t>
+  </si>
+  <si>
+    <t>α-amylase (EC 3.2.1.1)
+α-galactosidase (EC 3.2.1.22)
+amylopullulanase (EC 3.2.1.41)
+cyclomaltodextrinase (EC 3.2.1.54)
+branching enzyme (EC 2.4.1.18)
+4-α-glucanotransferase (EC 2.4.1.25)</t>
+  </si>
+  <si>
+    <t>mannosyl-oligosaccharide α-1,2-mannosidase (EC 3.2.1.113)
+mannosyl-oligosaccharide α-1,3-mannosidase (EC 3.2.1.-)
+mannosyl-oligosaccharide α-1,6-mannosidase (EC 3.2.1.-)
+α-mannosidase (EC 3.2.1.24)
+α-1,2-mannosidase (EC 3.2.1.-)
+α-1,3-mannosidase (EC 3.2.1.-)
+α-1,4-mannosidase (EC 3.2.1.-)
+mannosyl-1-phosphodiester α-1,P-mannosidase (EC 3.2.1.-)</t>
+  </si>
+  <si>
+    <t>pectate lyase (EC 4.2.2.2)
+exopolygalacturonate lyase (EC 4.2.2.9)
+thiopeptidoglycan lyase (EC 4.2.2.-)
+rhamnogalacturonan endolyase (EC 4.2.2.23)</t>
+  </si>
+  <si>
+    <t>mannosyl-oligosaccharide α-1,2-mannosidase (EC 3.2.1.113)
+α-mannosidase (EC 3.2.1.24)</t>
+  </si>
+  <si>
+    <t>Pectin degradation</t>
+  </si>
+  <si>
+    <t>Xylan degradation</t>
+  </si>
+  <si>
+    <t>Cellobiose and chitin degradation</t>
+  </si>
+  <si>
+    <t>Xylan and cellulose degradation</t>
+  </si>
+  <si>
+    <t>Highlight?</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Cellulose degradation</t>
+  </si>
+  <si>
+    <t>Mucin degradation</t>
+  </si>
+  <si>
+    <t>Blood cleaving</t>
+  </si>
+  <si>
+    <t>Blood mucin degradation</t>
+  </si>
+  <si>
+    <t>Fungal glycogen synthase</t>
+  </si>
+  <si>
+    <t>Peptidoglycan degradation</t>
+  </si>
+  <si>
+    <t>Eating bacteria? Cell wall breakdown during cell growth &amp; division?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,6 +577,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -491,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -502,6 +629,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -820,7 +954,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +974,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>75</v>
@@ -895,7 +1029,7 @@
         <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>60</v>
@@ -915,13 +1049,13 @@
         <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>27</v>
@@ -930,7 +1064,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -939,6 +1073,9 @@
       </c>
       <c r="C5" s="3" t="s">
         <v>60</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>60</v>
@@ -961,10 +1098,10 @@
         <v>68</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>27</v>
@@ -981,16 +1118,16 @@
         <v>73</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1000,8 +1137,11 @@
       <c r="C8" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="D8" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="E8" s="3" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>35</v>
@@ -1021,7 +1161,7 @@
         <v>58</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>29</v>
@@ -1035,19 +1175,19 @@
         <v>34</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1056,6 +1196,12 @@
       </c>
       <c r="C11" s="3" t="s">
         <v>63</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>35</v>
@@ -1075,7 +1221,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>36</v>
@@ -1092,7 +1238,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>60</v>
@@ -1132,16 +1278,16 @@
         <v>66</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>51</v>
       </c>
@@ -1150,6 +1296,9 @@
       </c>
       <c r="C16" s="3" t="s">
         <v>60</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>60</v>
@@ -1169,10 +1318,10 @@
         <v>67</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>35</v>
@@ -1201,7 +1350,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="3" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -1210,6 +1359,9 @@
       </c>
       <c r="C19" s="3" t="s">
         <v>60</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>60</v>
@@ -1229,10 +1381,10 @@
         <v>69</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>27</v>
@@ -1309,10 +1461,10 @@
         <v>70</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>29</v>
@@ -1358,7 +1510,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
@@ -1367,6 +1519,9 @@
       </c>
       <c r="C27" s="3" t="s">
         <v>60</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>60</v>
@@ -1403,25 +1558,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E19904D-E189-4D84-A406-27FFA4DB4AA2}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" customWidth="1"/>
+    <col min="5" max="5" width="40" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1429,306 +1586,420 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="E3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G3" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="E4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="G13" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E14" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="G14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="E15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F22" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1737,19 +2008,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB10AEF-13C5-47BF-802B-88E09E3AE0CB}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1757,25 +2030,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1783,14 +2059,19 @@
         <v>38</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1798,127 +2079,162 @@
         <v>38</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="E3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="E4" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>49</v>
+      <c r="C5" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="E6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G6" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F13" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Annotated for writing results
</commit_message>
<xml_diff>
--- a/dbcan/sig_cazy_info.xlsx
+++ b/dbcan/sig_cazy_info.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="620" documentId="8_{A1E0EE2A-CA9E-4781-BABE-4A2888B05358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC8B2B1B-0CBF-4A1F-AA40-A69AB1E5C289}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{88FD4827-B98C-4388-B407-BA95E8DEB523}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{88FD4827-B98C-4388-B407-BA95E8DEB523}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0420F783-523D-474B-9879-99329AEC3FC0}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,8 +1560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E19904D-E189-4D84-A406-27FFA4DB4AA2}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2010,8 +2010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB10AEF-13C5-47BF-802B-88E09E3AE0CB}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Summarized sig CAZyme taxa info
</commit_message>
<xml_diff>
--- a/dbcan/sig_cazy_info.xlsx
+++ b/dbcan/sig_cazy_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/dbcan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="620" documentId="8_{A1E0EE2A-CA9E-4781-BABE-4A2888B05358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC8B2B1B-0CBF-4A1F-AA40-A69AB1E5C289}"/>
+  <xr:revisionPtr revIDLastSave="624" documentId="8_{A1E0EE2A-CA9E-4781-BABE-4A2888B05358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CE9A239-FC29-44B6-87D5-A04571FF9A98}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{88FD4827-B98C-4388-B407-BA95E8DEB523}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{88FD4827-B98C-4388-B407-BA95E8DEB523}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -1560,8 +1560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E19904D-E189-4D84-A406-27FFA4DB4AA2}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2010,14 +2010,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB10AEF-13C5-47BF-802B-88E09E3AE0CB}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="38.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="39" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
   </cols>

</xml_diff>